<commit_message>
Fix menus excel sheet
</commit_message>
<xml_diff>
--- a/db/menus.xlsx
+++ b/db/menus.xlsx
@@ -8306,8 +8306,8 @@
       <c r="F181" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G181" s="1" t="s">
-        <v>14</v>
+      <c r="G181" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="H181" s="4">
         <v>25.0</v>
@@ -8350,8 +8350,8 @@
       <c r="F182" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G182" s="1" t="s">
-        <v>14</v>
+      <c r="G182" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="H182" s="4">
         <v>50.0</v>
@@ -8394,8 +8394,8 @@
       <c r="F183" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G183" s="1" t="s">
-        <v>14</v>
+      <c r="G183" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="H183" s="4">
         <v>75.0</v>
@@ -8438,8 +8438,8 @@
       <c r="F184" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G184" s="1" t="s">
-        <v>14</v>
+      <c r="G184" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="H184" s="1" t="s">
         <v>15</v>
@@ -8482,8 +8482,8 @@
       <c r="F185" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G185" s="1" t="s">
-        <v>14</v>
+      <c r="G185" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="H185" s="1" t="s">
         <v>16</v>
@@ -8526,8 +8526,8 @@
       <c r="F186" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G186" s="1" t="s">
-        <v>14</v>
+      <c r="G186" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="H186" s="1" t="s">
         <v>17</v>
@@ -8570,8 +8570,8 @@
       <c r="F187" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G187" s="1" t="s">
-        <v>14</v>
+      <c r="G187" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="H187" s="1" t="s">
         <v>18</v>

</xml_diff>